<commit_message>
Atualizador do tipo de dados da coluna
</commit_message>
<xml_diff>
--- a/Codes/data_table1.xlsx
+++ b/Codes/data_table1.xlsx
@@ -531,15 +531,23 @@
           <t>BCFF11.SA</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>BRL</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>71.98999999999999</v>
+        <v>71.91</v>
       </c>
       <c r="F3" t="n">
         <v>73.1842</v>
@@ -547,7 +555,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>3.4722424</v>
+        <v>3.468384</v>
       </c>
       <c r="J3" t="inlineStr"/>
     </row>
@@ -573,7 +581,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>4.44</v>
+        <v>4.42</v>
       </c>
       <c r="F4" t="n">
         <v>4.4962</v>
@@ -585,7 +593,7 @@
         <v>0.084300004</v>
       </c>
       <c r="I4" t="n">
-        <v>5.2235293</v>
+        <v>5.2</v>
       </c>
       <c r="J4" t="n">
         <v>6.022</v>

</xml_diff>